<commit_message>
Priority update in ProductSearchPageTest
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testData.xlsx
+++ b/src/test/resources/testdata/testData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>firstname</t>
   </si>
@@ -398,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -443,28 +443,6 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>